<commit_message>
CV Hoja 7 corrección errores
</commit_message>
<xml_diff>
--- a/FALEC-w1-core-web/WebContent/reportes/FALECPV-listaproveedor.xlsx
+++ b/FALEC-w1-core-web/WebContent/reportes/FALECPV-listaproveedor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10307"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/System/Volumes/Data/projects/gitrepositorio/FacturaElectronica-App/FALEC-w1-core-web/WebContent/reportes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7AFC86C3-FEEE-4B47-953E-F62B34174631}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC84F5F-360F-2644-B6DD-5FFE361B81D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="2600" windowWidth="32760" windowHeight="22260"/>
+    <workbookView xWindow="4760" yWindow="2600" windowWidth="32760" windowHeight="22260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -162,14 +162,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -485,11 +485,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>